<commit_message>
updates to figures and results
</commit_message>
<xml_diff>
--- a/data/tr010_primers.xlsx
+++ b/data/tr010_primers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\706194\projects\ribo-accum-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF0136-844B-460E-A955-8A93B35C1D1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09DD504-6640-435C-80DA-AC23EF4B2433}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="1335" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1905" windowWidth="19245" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="129">
   <si>
     <t>47S F1R1</t>
   </si>
@@ -299,27 +299,6 @@
     <t>symbol_ext</t>
   </si>
   <si>
-    <t>RNA45S ETS</t>
-  </si>
-  <si>
-    <t>RNA47S ETS</t>
-  </si>
-  <si>
-    <t>RNA45S ITS</t>
-  </si>
-  <si>
-    <t>RNA5-8S</t>
-  </si>
-  <si>
-    <t>RNA28S</t>
-  </si>
-  <si>
-    <t>RNA18S</t>
-  </si>
-  <si>
-    <t>RNA5S</t>
-  </si>
-  <si>
     <t>UBTF [1,4]</t>
   </si>
   <si>
@@ -432,6 +411,15 @@
   </si>
   <si>
     <t>Lambda KIT</t>
+  </si>
+  <si>
+    <t>rRNA47S ETS</t>
+  </si>
+  <si>
+    <t>rRNA45S ETS</t>
+  </si>
+  <si>
+    <t>rRNA45S ITS</t>
   </si>
 </sst>
 </file>
@@ -772,7 +760,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -823,7 +811,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
@@ -844,7 +832,7 @@
         <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="I2" t="s">
         <v>58</v>
@@ -858,7 +846,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>50</v>
@@ -879,7 +867,7 @@
         <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="I3" t="s">
         <v>59</v>
@@ -893,7 +881,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -914,7 +902,7 @@
         <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="I4" t="s">
         <v>58</v>
@@ -928,7 +916,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>24</v>
@@ -949,7 +937,7 @@
         <v>68</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>60</v>
@@ -963,7 +951,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -984,7 +972,7 @@
         <v>61</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>62</v>
@@ -998,7 +986,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>30</v>
@@ -1019,7 +1007,7 @@
         <v>63</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>64</v>
@@ -1033,7 +1021,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -1054,7 +1042,7 @@
         <v>67</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>65</v>
@@ -1091,7 +1079,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
@@ -1141,7 +1129,7 @@
         <v>73</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>74</v>
@@ -1170,7 +1158,7 @@
         <v>75</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>74</v>
@@ -1265,7 +1253,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>79</v>
@@ -1274,13 +1262,13 @@
         <v>79</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1288,10 +1276,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C18" s="4">
         <v>43883</v>
@@ -1308,10 +1296,10 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E19" s="4">
         <v>43970</v>
@@ -1328,13 +1316,13 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F20" s="5">
         <v>33970</v>
@@ -1348,13 +1336,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F21" s="5">
         <v>18660</v>
@@ -1371,10 +1359,10 @@
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F22" s="5">
         <v>23012</v>
@@ -1388,10 +1376,10 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E23" s="4">
         <v>43912</v>
@@ -1408,10 +1396,10 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E24" s="4">
         <v>43900</v>
@@ -1428,10 +1416,10 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E25" s="4">
         <v>44022</v>
@@ -1448,10 +1436,10 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E26" s="4">
         <v>43884</v>
@@ -1468,13 +1456,13 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E27" s="5">
         <v>45323</v>
@@ -1488,10 +1476,10 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D28" s="4">
         <v>43873</v>
@@ -1508,10 +1496,10 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D29" s="4">
         <v>43917</v>
@@ -1528,10 +1516,10 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D30" s="4">
         <v>44027</v>
@@ -1548,10 +1536,10 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D31" s="4">
         <v>43847</v>
@@ -1560,7 +1548,7 @@
         <v>42767</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1568,10 +1556,10 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D32" s="4">
         <v>43949</v>
@@ -1588,13 +1576,13 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E33" s="5">
         <v>30317</v>

</xml_diff>